<commit_message>
S1_TC21, 23, 25 (Changes)
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 1/S1_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 1/S1_TestCases_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawe\git\tb-ttap-brivge-v2-fatin\Excel Files\Scenario 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9547CA6D-C536-4052-9CAA-D3F3DB4985F9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{52EE57C0-DEA2-4F80-B937-1E3370F36D9C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="40" firstSheet="35" tabRatio="547" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="31" firstSheet="31" tabRatio="547" windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="AutoIncrement" r:id="rId1" sheetId="1"/>
@@ -19437,8 +19437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C995E7-3C41-44BE-92B7-C62CA640336D}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D19:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20088,7 +20088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B4C763-E53F-4B86-9C00-751B722E35A6}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TC53 and TC54 FIX
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 1/S1_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 1/S1_TestCases_Data.xlsx
@@ -753,7 +753,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6908" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6909" uniqueCount="572">
   <si>
     <t>No</t>
   </si>
@@ -2496,6 +2496,9 @@
   </si>
   <si>
     <t>rsCS202-2311001-01</t>
+  </si>
+  <si>
+    <t>rsCS102-2311002-01</t>
   </si>
 </sst>
 </file>
@@ -31932,7 +31935,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>502</v>
+        <v>571</v>
       </c>
       <c r="B2" t="s">
         <v>570</v>

</xml_diff>